<commit_message>
Report and backlog update
Commit reports
</commit_message>
<xml_diff>
--- a/ProductBacklog/Product-Backlog.xlsx
+++ b/ProductBacklog/Product-Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="210" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="270" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,19 +358,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,11 +569,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45870592"/>
-        <c:axId val="167699584"/>
+        <c:axId val="42873344"/>
+        <c:axId val="292843456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45870592"/>
+        <c:axId val="42873344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167699584"/>
+        <c:crossAx val="292843456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,7 +614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167699584"/>
+        <c:axId val="292843456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45870592"/>
+        <c:crossAx val="42873344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,19 +1005,19 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="28"/>
+      <c r="F4" s="24"/>
       <c r="G4" t="s">
         <v>6</v>
       </c>
@@ -1284,20 +1284,20 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="19">
+      <c r="B17" s="7">
         <v>13</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="9">
         <v>5</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="10">
         <v>20</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>31</v>
+      <c r="F17" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1403,37 +1403,37 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="19">
+      <c r="B24" s="7">
         <v>20</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="9">
         <v>8</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="10">
         <v>6</v>
       </c>
-      <c r="F24" s="18" t="s">
-        <v>31</v>
+      <c r="F24" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="22">
+      <c r="B25" s="25">
         <v>21</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="27">
         <v>8</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="28">
         <v>10</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>31</v>
+      <c r="F25" s="26" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Backlog for sprint 2 is updated
completed tasks and inprogress tasks are added
</commit_message>
<xml_diff>
--- a/ProductBacklog/Product-Backlog.xlsx
+++ b/ProductBacklog/Product-Backlog.xlsx
@@ -569,11 +569,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42873344"/>
-        <c:axId val="292843456"/>
+        <c:axId val="290568192"/>
+        <c:axId val="214617472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42873344"/>
+        <c:axId val="290568192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292843456"/>
+        <c:crossAx val="214617472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,7 +614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292843456"/>
+        <c:axId val="214617472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42873344"/>
+        <c:crossAx val="290568192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,37 +1077,37 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="19">
+      <c r="B8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="13">
         <v>2</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="14">
         <v>10</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>31</v>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="19">
+      <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="9">
         <v>2</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="10">
         <v>6</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>31</v>
+      <c r="F9" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="J9" t="s">
         <v>32</v>
@@ -1169,20 +1169,20 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="11">
         <v>8</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="13">
         <v>3</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="14">
         <v>24</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>10</v>
+      <c r="F12" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="I12" t="s">
         <v>36</v>
@@ -1192,20 +1192,20 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="19">
+      <c r="B13" s="7">
         <v>9</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="9">
         <v>3</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="10">
         <v>10</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>31</v>
+      <c r="F13" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="I13" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Begin to work on login process
</commit_message>
<xml_diff>
--- a/ProductBacklog/Product-Backlog.xlsx
+++ b/ProductBacklog/Product-Backlog.xlsx
@@ -569,11 +569,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="290568192"/>
-        <c:axId val="214617472"/>
+        <c:axId val="59679872"/>
+        <c:axId val="59681792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290568192"/>
+        <c:axId val="59679872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214617472"/>
+        <c:crossAx val="59681792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,7 +614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214617472"/>
+        <c:axId val="59681792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290568192"/>
+        <c:crossAx val="59679872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -972,7 +972,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,20 +1238,20 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="19">
+      <c r="B15" s="7">
         <v>11</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="9">
         <v>4</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="10">
         <v>10</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>31</v>
+      <c r="F15" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="I15" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Update for sprint 2
Product backlog and sprint backlog 2  is updated
</commit_message>
<xml_diff>
--- a/ProductBacklog/Product-Backlog.xlsx
+++ b/ProductBacklog/Product-Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="270" windowWidth="20115" windowHeight="7875"/>
+    <workbookView xWindow="240" yWindow="330" windowWidth="20115" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +210,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -315,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -369,6 +375,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -554,6 +568,9 @@
                 <c:pt idx="1">
                   <c:v>19</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -569,11 +586,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="59679872"/>
-        <c:axId val="59681792"/>
+        <c:axId val="44929024"/>
+        <c:axId val="92701824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59679872"/>
+        <c:axId val="44929024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59681792"/>
+        <c:crossAx val="92701824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -614,18 +631,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59681792"/>
+        <c:axId val="92701824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59679872"/>
+        <c:crossAx val="44929024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -651,16 +687,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -971,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,24 +1126,24 @@
         <v>10</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="11">
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="13">
         <v>2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="14">
         <v>6</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>10</v>
+      <c r="F9" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="J9" t="s">
         <v>32</v>
@@ -1190,22 +1226,25 @@
       <c r="J12">
         <v>14</v>
       </c>
+      <c r="K12">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="29">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="31">
         <v>3</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="32">
         <v>10</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>10</v>
+      <c r="F13" s="30" t="s">
+        <v>31</v>
       </c>
       <c r="I13" t="s">
         <v>37</v>
@@ -1284,37 +1323,37 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="B17" s="11">
         <v>13</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="13">
         <v>5</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="14">
         <v>20</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
+        <v>14</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="9">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>8</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="19">
-        <v>14</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="20">
-        <v>5</v>
-      </c>
-      <c r="E18" s="21">
-        <v>8</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1403,20 +1442,20 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7">
+      <c r="B24" s="11">
         <v>20</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="13">
         <v>8</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="14">
         <v>6</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>10</v>
+      <c r="F24" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>